<commit_message>
Added test cases to verizon.com
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1183904-F303-49BA-A602-C11D4E2EE085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EDF6E8-A377-4251-A564-A14B76855BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Brands" sheetId="1" r:id="rId1"/>
+    <sheet name="Accessories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Assertions</t>
   </si>
@@ -53,6 +54,18 @@
   </si>
   <si>
     <t>Business Google Smartphones</t>
+  </si>
+  <si>
+    <t>Bundle Eligible Cases</t>
+  </si>
+  <si>
+    <t>Bundle Eligible Screen Protectors</t>
+  </si>
+  <si>
+    <t>iPad Cases</t>
+  </si>
+  <si>
+    <t>Tablet Accessories</t>
   </si>
 </sst>
 </file>
@@ -414,9 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -459,4 +470,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3CAF5F-D7B8-4887-874E-DC4EC110B401}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test cases to verizon.
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/test_data.xlsx
+++ b/com.verizon/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.verizon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EDF6E8-A377-4251-A564-A14B76855BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A109B-6867-49F4-9B20-609671D61BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="0" windowWidth="17140" windowHeight="14320" activeTab="1" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Assertions</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Tablet Accessories</t>
+  </si>
+  <si>
+    <t>Cases &amp; Protection</t>
   </si>
 </sst>
 </file>
@@ -108,9 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3CAF5F-D7B8-4887-874E-DC4EC110B401}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,6 +516,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>